<commit_message>
working on Uplacerbare #73
</commit_message>
<xml_diff>
--- a/node-red/konteringsregler/Skabelon, KMD.xlsx
+++ b/node-red/konteringsregler/Skabelon, KMD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Christian S. Leonhardt\Må slettes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dq28777\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C330464-5801-4844-B96A-D0A710F4CFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736F01AB-98B8-4F95-8E28-B2B2DCCB594E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regler" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="99">
   <si>
     <t>Starter med</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Betalingsservice</t>
   </si>
   <si>
-    <t>Advisliste</t>
-  </si>
-  <si>
     <t>Assentoft</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>Kontant transaktion Assentoftskolens kantine</t>
   </si>
   <si>
-    <t>match_regel</t>
-  </si>
-  <si>
     <t>Posteringstype</t>
   </si>
   <si>
@@ -316,9 +310,6 @@
     <t>Undtagelser, dvs bankposteringer som bliver håndteret af andre snitflader, håndteres ved at angive bankkontoens kontering i reglen. Skriv evt. snitfladens navn i notatfeltet.</t>
   </si>
   <si>
-    <t>Egen snitflade</t>
-  </si>
-  <si>
     <t>Bruges til pensionsbidrag</t>
   </si>
   <si>
@@ -335,6 +326,12 @@
   </si>
   <si>
     <t>Konteringsregler behøver ikke at være anført med beløbsafgrænsning, men muligheden er der.</t>
+  </si>
+  <si>
+    <t>Bankkonto</t>
+  </si>
+  <si>
+    <t>Undtagelse - Artskonto = statuskonto registreret i FOBI</t>
   </si>
 </sst>
 </file>
@@ -675,7 +672,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -799,6 +796,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -852,7 +858,7 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -876,13 +882,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -895,11 +894,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="20 % - Farve1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -953,7 +974,45 @@
     <cellStyle name="Ugyldig" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Ugyldig 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -984,91 +1043,25 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1126,14 +1119,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="medium">
           <color auto="1"/>
@@ -1150,14 +1135,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1172,25 +1149,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D7D72FC-61B6-4536-B926-DBAD181DF54C}" name="Tabel13" displayName="Tabel13" ref="A1:M9" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22">
-  <autoFilter ref="A1:M9" xr:uid="{4D7D72FC-61B6-4536-B926-DBAD181DF54C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M9">
-    <sortCondition sortBy="cellColor" ref="A1:A9" dxfId="21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D7D72FC-61B6-4536-B926-DBAD181DF54C}" name="Tabel13" displayName="Tabel13" ref="A1:L9" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:L9" xr:uid="{4D7D72FC-61B6-4536-B926-DBAD181DF54C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K9">
+    <sortCondition sortBy="cellColor" ref="A1:A9" dxfId="9"/>
   </sortState>
-  <tableColumns count="13">
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{0F649F2C-72DC-4FBF-B32C-117DBCC7BAF6}" name="Reference"/>
-    <tableColumn id="2" xr3:uid="{920C1AB9-E171-4647-B912-7A784C13F1E9}" name="Advisliste"/>
     <tableColumn id="3" xr3:uid="{90073830-B7C1-4976-A1B7-DA083667838D}" name="Afsender"/>
     <tableColumn id="4" xr3:uid="{31FEE8AB-882D-4817-96D3-50F51737D875}" name="Posteringstype"/>
-    <tableColumn id="5" xr3:uid="{8706A404-FD4E-4C92-8496-4B92BBFCCD1F}" name="match_regel"/>
-    <tableColumn id="6" xr3:uid="{203994D9-55C9-4053-9C50-57B9F18CB2C7}" name="Beløb1" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{E1D3D2E9-6201-443D-81A4-9CE906D492F2}" name="Beløb2" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{203994D9-55C9-4053-9C50-57B9F18CB2C7}" name="Beløb1" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{E1D3D2E9-6201-443D-81A4-9CE906D492F2}" name="Beløb2" dataDxfId="14"/>
     <tableColumn id="14" xr3:uid="{44187BD2-003A-454C-B409-77969467EB45}" name="beløb_regel"/>
-    <tableColumn id="8" xr3:uid="{5CBA1862-E86B-4FCC-B0E2-29154EA58AE0}" name="Posteringstekst" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{B6825CEB-3291-4A75-8B9E-F6F8F723B4D3}" name="Artskonto" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{BEBFE1C8-2C04-455A-8F5A-52451AA908D9}" name="PSP-element" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{5CBA1862-E86B-4FCC-B0E2-29154EA58AE0}" name="Posteringstekst" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{B6825CEB-3291-4A75-8B9E-F6F8F723B4D3}" name="Artskonto" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{BEBFE1C8-2C04-455A-8F5A-52451AA908D9}" name="PSP-element" dataDxfId="11"/>
     <tableColumn id="11" xr3:uid="{C2951F01-8A28-4320-A216-A82D58E05C02}" name="SIO"/>
-    <tableColumn id="7" xr3:uid="{D80C2040-2A24-4D45-B81A-EC0EA649DDA9}" name="Notat" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{D80C2040-2A24-4D45-B81A-EC0EA649DDA9}" name="Notat" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{0F216EE7-E398-4918-8314-110D9ACE5766}" name="Bankkonto" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1459,289 +1435,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N777"/>
+  <dimension ref="A1:P777"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.75" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="57.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="76.5" style="6" customWidth="1"/>
-    <col min="14" max="14" width="0" style="2" hidden="1"/>
-    <col min="15" max="16384" width="9" style="2" hidden="1"/>
+    <col min="1" max="1" width="19.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
+      <c r="B1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="12" t="s">
+      <c r="J1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="21"/>
-      <c r="H2"/>
-      <c r="J2" s="14">
+      <c r="E2" s="16"/>
+      <c r="F2"/>
+      <c r="H2" s="11">
         <v>40000000</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="I2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" s="15">
+        <v>3000000</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="L2"/>
-      <c r="M2" s="10"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3"/>
-      <c r="C3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="20">
-        <v>3000000</v>
-      </c>
-      <c r="G3" s="21"/>
-      <c r="H3" t="s">
+      <c r="H3" s="11">
+        <v>95914002</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="15">
+        <v>167</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="14">
-        <v>95914002</v>
-      </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4"/>
-      <c r="B4" s="16"/>
-      <c r="C4"/>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="20">
-        <v>167</v>
-      </c>
-      <c r="G4" s="21"/>
-      <c r="H4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" s="14">
+      <c r="G4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="11">
         <v>79000000</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="I4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L4"/>
-      <c r="M4" s="10"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J4"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="20">
+      <c r="D5" s="15">
         <v>200</v>
       </c>
-      <c r="G5" s="21">
+      <c r="E5" s="16">
         <v>1100</v>
       </c>
-      <c r="H5" t="s">
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="14">
+      <c r="H5" s="11">
         <v>91407008</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5"/>
-      <c r="M5" s="10"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>67</v>
+      <c r="I5" s="12"/>
+      <c r="J5"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6"/>
-      <c r="I6" s="8" t="s">
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6"/>
+      <c r="G6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="11">
+        <v>79000000</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7"/>
+      <c r="G7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="14">
-        <v>79000000</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7"/>
-      <c r="I7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="14">
+      <c r="H7" s="11">
         <v>72000000</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="I7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="10"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J7" s="11"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8"/>
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
       <c r="C8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21"/>
-      <c r="H8"/>
-      <c r="I8" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="J8" s="17">
+        <v>20</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8"/>
+      <c r="G8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="14">
         <v>72000000</v>
       </c>
-      <c r="K8" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9"/>
-      <c r="I9" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" s="17">
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9"/>
+      <c r="G9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="14">
         <v>90540000</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="L9"/>
-      <c r="M9" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2"/>
+      <c r="I9" s="12"/>
+      <c r="J9"/>
+      <c r="K9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2"/>
     <row r="17" x14ac:dyDescent="0.2"/>
     <row r="18" x14ac:dyDescent="0.2"/>
     <row r="19" x14ac:dyDescent="0.2"/>
@@ -2505,31 +2452,26 @@
     <row r="777" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="22" type="noConversion"/>
-  <conditionalFormatting sqref="B9 E9 A2:M8 A10:M1048576">
-    <cfRule type="expression" dxfId="1" priority="30">
-      <formula>OR(LEFT($A2,1)="#",LEFT($B2,1)="#",LEFT($C2,1)="#",LEFT($D2,1)="#")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9 C9:D9 F9:M9">
-    <cfRule type="expression" dxfId="0" priority="37">
-      <formula>OR(LEFT(#REF!,1)="#",LEFT($A9,1)="#",LEFT($C9,1)="#",LEFT($D9,1)="#")</formula>
+  <conditionalFormatting sqref="A2:L777">
+    <cfRule type="expression" dxfId="1" priority="43">
+      <formula>OR(LEFT($A2,1)="#",LEFT($B2,1)="#",LEFT($C2,1)="#")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="J2:J7 J9:J1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="H2:H7 H9:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>10000000</formula1>
       <formula2>99500000</formula2>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="J1" xr:uid="{0201F26A-5C3B-4A9E-B8E0-4F0EFEC94065}"/>
-    <dataValidation type="decimal" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ændr beløb" error="Du kan kun indtaste et beløb mellem -999.999 og 999.999" sqref="F2 G2:G3 F4:G9" xr:uid="{8F8CD826-C7FE-4AD7-809F-D67FB26120C9}">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="H1" xr:uid="{0201F26A-5C3B-4A9E-B8E0-4F0EFEC94065}"/>
+    <dataValidation type="decimal" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ændr beløb" error="Du kan kun indtaste et beløb mellem -999.999 og 999.999" sqref="D2 E2:E3 D4:E9" xr:uid="{8F8CD826-C7FE-4AD7-809F-D67FB26120C9}">
       <formula1>-999999</formula1>
       <formula2>999999</formula2>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ændr beløb" error="Du kan kun indtaste et beløb mellem -999.999 og 999.999" sqref="F3" xr:uid="{0DBF8480-C654-4D74-B3F8-1E04130436A8}">
+    <dataValidation type="decimal" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ændr beløb" error="Du kan kun indtaste et beløb mellem -999.999 og 999.999" sqref="D3" xr:uid="{0DBF8480-C654-4D74-B3F8-1E04130436A8}">
       <formula1>-9999999</formula1>
       <formula2>9999999</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ændr beløb" error="Du kan kun indtaste et beløb mellem -999.999 og 999.999" sqref="F10:G1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="whole" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ændr beløb" error="Du kan kun indtaste et beløb mellem -999.999 og 999.999" sqref="D10:E1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>-999999</formula1>
       <formula2>999999</formula2>
     </dataValidation>
@@ -2541,30 +2483,24 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fejl" error="Ugyldig værdi" xr:uid="{DE70A504-CEC8-44E2-8924-A04333B42D89}">
           <x14:formula1>
             <xm:f>Validering!$C$2:$C$30</xm:f>
           </x14:formula1>
-          <xm:sqref>D22:D1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
-          <x14:formula1>
-            <xm:f>Validering!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>C22:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>Validering!$A$7:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fejl" error="Ugyldig værdi" xr:uid="{F5947B76-C8CE-44A2-A162-8CE61EB65A2E}">
           <x14:formula1>
             <xm:f>Validering!$C$2:$C$31</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D21</xm:sqref>
+          <xm:sqref>C2:C21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2584,72 +2520,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2676,16 +2612,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2693,7 +2629,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>271</v>
@@ -2704,13 +2640,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>184</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2718,7 +2654,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>225</v>
@@ -2729,21 +2665,21 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>525</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>121</v>
@@ -2751,10 +2687,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>409</v>
@@ -2762,10 +2698,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8">
         <v>251</v>
@@ -2773,10 +2709,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9">
         <v>433</v>
@@ -2784,10 +2720,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D10">
         <v>16</v>
@@ -2795,7 +2731,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2803,7 +2739,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>366</v>
@@ -2811,18 +2747,18 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13">
         <v>158</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14">
         <v>283</v>
@@ -2830,18 +2766,18 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>102</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D16">
         <v>250</v>
@@ -2849,40 +2785,40 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17">
         <v>231</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18">
         <v>341</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D19">
         <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20">
         <v>253</v>
@@ -2890,7 +2826,7 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D21">
         <v>74</v>
@@ -2898,18 +2834,18 @@
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D22">
         <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23">
         <v>326</v>
@@ -2917,29 +2853,29 @@
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D24">
         <v>216</v>
       </c>
       <c r="E24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25">
         <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26">
         <v>66</v>
@@ -2947,7 +2883,7 @@
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D27">
         <v>81</v>
@@ -2955,18 +2891,18 @@
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D28">
         <v>358</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D29">
         <v>334</v>
@@ -2974,7 +2910,7 @@
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D30">
         <v>333</v>
@@ -2982,7 +2918,7 @@
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D31">
         <v>272</v>

</xml_diff>